<commit_message>
add parameters for VEGF-B and PlGF reactions (PlGF parameters will be added after issue #3)
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0DEFE68-C73C-DE4D-8141-E69AC9AD96C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F8B40E-DB3D-D744-A0E2-910328E08A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="120">
   <si>
     <t>Parameter</t>
   </si>
@@ -345,6 +345,57 @@
   </si>
   <si>
     <t>Dissociation rate of VEGFR1:NRP1 complex</t>
+  </si>
+  <si>
+    <t>konVBR1</t>
+  </si>
+  <si>
+    <t>konVBN1</t>
+  </si>
+  <si>
+    <t>konPlR1</t>
+  </si>
+  <si>
+    <t>konPlN1</t>
+  </si>
+  <si>
+    <t>koffVBR1</t>
+  </si>
+  <si>
+    <t>koffVBN1</t>
+  </si>
+  <si>
+    <t>koffPlR1</t>
+  </si>
+  <si>
+    <t>koffPlN1</t>
+  </si>
+  <si>
+    <t>Association rate of VEGF-B binding to VEGFR1</t>
+  </si>
+  <si>
+    <t>Dissociation rate of VEGF-B bound to VEGFR1</t>
+  </si>
+  <si>
+    <t>Association rate of VEGF-B binding to NRP1</t>
+  </si>
+  <si>
+    <t>Dissociation rate of VEGF-B bound to NRP1</t>
+  </si>
+  <si>
+    <t>Association rate of PlGF binding to VEGFR1</t>
+  </si>
+  <si>
+    <t>Dissociation rate of PlGF bound to VEGFR1</t>
+  </si>
+  <si>
+    <t>Association rate of PlGF binding to NRP1</t>
+  </si>
+  <si>
+    <t>Dissociation rate of PlGF bound to NRP1</t>
+  </si>
+  <si>
+    <t>Hoffman et al., 2013</t>
   </si>
 </sst>
 </file>
@@ -919,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DEB865-22A6-6340-B754-943FBB9E2F98}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,377 +1332,505 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="C21" s="2">
-        <v>1100</v>
+        <v>158000</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="C22" s="2">
-        <v>2.6999999999999999E-5</v>
+        <v>9.145E-5</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="C23" s="2">
-        <v>12000</v>
+        <v>126000</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C24" s="2">
-        <v>3.9999999999999998E-6</v>
+        <v>1.94E-4</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="2">
-        <v>204000</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="2">
-        <v>3.035E-4</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="2">
-        <v>162000</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>25</v>
+        <v>110</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="2">
-        <v>3.8299999999999999E-4</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C28" s="2"/>
       <c r="D28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2">
-        <v>169000</v>
+        <v>1100</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C30" s="2">
-        <v>3.77E-4</v>
+        <v>2.6999999999999999E-5</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C31" s="2">
-        <v>214000</v>
+        <v>12000</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C32" s="2">
-        <v>5.8100000000000001E-3</v>
+        <v>3.9999999999999998E-6</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C33" s="2">
-        <v>1300</v>
+        <v>204000</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C34" s="2">
-        <v>2.8999999999999998E-3</v>
+        <v>3.035E-4</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="2">
+        <v>162000</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3.8299999999999999E-4</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="2">
+        <v>169000</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3.77E-4</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="2">
+        <v>214000</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="2">
+        <v>5.8100000000000001E-3</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1300</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C43" s="2">
         <f>(336000+325000)/2</f>
         <v>330500</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C44" s="2">
         <f>(0.000604+0.000905)/2</f>
         <v>7.5449999999999996E-4</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="D44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C45" s="2">
         <v>219000</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C46" s="2">
         <v>3.0300000000000001E-5</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="5" t="s">
+      <c r="D46" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C47" s="2">
         <v>173000</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C48" s="2">
         <v>3.2099999999999998E-7</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="5" t="s">
+      <c r="D48" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C49" s="2">
         <v>250000</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="50" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B50" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C50" s="8">
         <v>4.4999999999999999E-4</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="10" t="s">
+      <c r="D50" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
use PlGF:VEGFR1 binding rates measured by Shobhan
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F8B40E-DB3D-D744-A0E2-910328E08A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8F0386-701E-574A-893B-6CB0F393EF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -973,7 +973,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1405,12 +1405,14 @@
       <c r="B25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>57900</v>
+      </c>
       <c r="D25" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1420,12 +1422,14 @@
       <c r="B26" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2">
+        <v>2.6900000000000001E-6</v>
+      </c>
       <c r="D26" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
use PlGF:NRP1 binding rates from `Clegg et al., 2017` and `Hoffman et al., 2013`
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8F0386-701E-574A-893B-6CB0F393EF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC7AA3-997C-D044-A61E-766838069799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -395,7 +395,7 @@
     <t>Dissociation rate of PlGF bound to NRP1</t>
   </si>
   <si>
-    <t>Hoffman et al., 2013</t>
+    <t>Clegg et al., 2017 &amp; Hoffman et al., 2013</t>
   </si>
 </sst>
 </file>
@@ -973,7 +973,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1439,7 +1439,9 @@
       <c r="B27" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>10000</v>
+      </c>
       <c r="D27" s="3" t="s">
         <v>45</v>
       </c>
@@ -1454,7 +1456,9 @@
       <c r="B28" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="D28" s="3" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
add concentration of complexes to parameter list
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC7AA3-997C-D044-A61E-766838069799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5805CB-F9CB-2C4B-865C-F7A66706C566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="158">
   <si>
     <t>Parameter</t>
   </si>
@@ -396,6 +396,120 @@
   </si>
   <si>
     <t>Clegg et al., 2017 &amp; Hoffman et al., 2013</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-A:VEGFR1</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-A:VEGFR2</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-A:NRP1</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-A:VEGFR2:NRP1</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-A:PDGFRα</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-A:PDGFRβ</t>
+  </si>
+  <si>
+    <t>VA_R1</t>
+  </si>
+  <si>
+    <t>VA_R2</t>
+  </si>
+  <si>
+    <t>VA_N1</t>
+  </si>
+  <si>
+    <t>VA_R2_N1</t>
+  </si>
+  <si>
+    <t>VA_PDRa</t>
+  </si>
+  <si>
+    <t>VA_PDRb</t>
+  </si>
+  <si>
+    <t>VB_R1</t>
+  </si>
+  <si>
+    <t>VB_N1</t>
+  </si>
+  <si>
+    <t>Pl_R1</t>
+  </si>
+  <si>
+    <t>Pl_N1</t>
+  </si>
+  <si>
+    <t>PDAA_R2</t>
+  </si>
+  <si>
+    <t>PDAA_PDRa</t>
+  </si>
+  <si>
+    <t>PDAB_R2</t>
+  </si>
+  <si>
+    <t>PDAB_PDRa</t>
+  </si>
+  <si>
+    <t>PDAB_PDRb</t>
+  </si>
+  <si>
+    <t>PDBB_R2</t>
+  </si>
+  <si>
+    <t>PDBB_PDRa</t>
+  </si>
+  <si>
+    <t>PDBB_PDRb</t>
+  </si>
+  <si>
+    <t>R1_N1</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-B:VEGFR1</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-B:PlGF</t>
+  </si>
+  <si>
+    <t>Concentration of PlGF:VEGFR1</t>
+  </si>
+  <si>
+    <t>Concentration of PlGF:NRP1</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-AA:VEGFR2</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-AA:PDGFRα</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-AB:VEGFR2</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-AB:PDGFRα</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-AB:PDGFRβ</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-BB:VEGFR2</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-BB:PDGFRβ</t>
+  </si>
+  <si>
+    <t>Concentration of PDGF-BB:PDGFRα</t>
+  </si>
+  <si>
+    <t>Concentration of VEGFR1:NRP1</t>
   </si>
 </sst>
 </file>
@@ -970,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DEB865-22A6-6340-B754-943FBB9E2F98}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1162,509 +1276,509 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="C11" s="2">
-        <v>11370000</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="C12" s="2">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>3</v>
+        <v>128</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="C13" s="2">
-        <v>4650000</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="C14" s="2">
-        <v>7.6999999999999996E-4</v>
+        <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>73</v>
+        <v>130</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="C15" s="2">
-        <v>1260000</v>
+        <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>82</v>
+        <v>131</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="C16" s="2">
-        <v>3.48E-3</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="C17" s="2">
-        <v>100000000000000</v>
+        <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="C18" s="2">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="C19" s="2">
-        <v>31000000000000</v>
+        <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="C20" s="2">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C21" s="2">
-        <v>158000</v>
+        <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="C22" s="2">
-        <v>9.145E-5</v>
+        <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="C23" s="2">
-        <v>126000</v>
+        <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="C24" s="2">
-        <v>1.94E-4</v>
+        <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="C25" s="2">
-        <v>57900</v>
+        <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="C26" s="2">
-        <v>2.6900000000000001E-6</v>
+        <v>0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="C27" s="2">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="C28" s="2">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="C29" s="2">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C30" s="2">
-        <v>2.6999999999999999E-5</v>
+        <v>11370000</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2">
-        <v>12000</v>
+        <v>1E-4</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C32" s="2">
-        <v>3.9999999999999998E-6</v>
+        <v>4650000</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C33" s="2">
-        <v>204000</v>
+        <v>7.6999999999999996E-4</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>4</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="C34" s="2">
-        <v>3.035E-4</v>
+        <v>1260000</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>91</v>
+        <v>19</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="C35" s="2">
-        <v>162000</v>
+        <v>3.48E-3</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C36" s="2">
-        <v>3.8299999999999999E-4</v>
+        <v>100000000000000</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C37" s="2">
-        <v>169000</v>
+        <v>1E-3</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C38" s="2">
-        <v>3.77E-4</v>
+        <v>31000000000000</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C39" s="2">
-        <v>214000</v>
+        <v>1E-3</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C40" s="2">
-        <v>5.8100000000000001E-3</v>
+        <v>158000</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>60</v>
@@ -1672,173 +1786,496 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="C41" s="2">
-        <v>1300</v>
+        <v>9.145E-5</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C42" s="2">
-        <v>2.8999999999999998E-3</v>
+        <v>126000</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1.94E-4</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="2">
+        <v>57900</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2.6900000000000001E-6</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1100</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2.6999999999999999E-5</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="2">
+        <v>12000</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="2">
+        <v>204000</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3.035E-4</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="2">
+        <v>162000</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="2">
+        <v>3.8299999999999999E-4</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="2">
+        <v>169000</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="2">
+        <v>3.77E-4</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="2">
+        <v>214000</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="2">
+        <v>5.8100000000000001E-3</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1300</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C62" s="2">
         <f>(336000+325000)/2</f>
         <v>330500</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E62" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C63" s="2">
         <f>(0.000604+0.000905)/2</f>
         <v>7.5449999999999996E-4</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C64" s="2">
         <v>219000</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E64" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C65" s="2">
         <v>3.0300000000000001E-5</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C66" s="2">
         <v>173000</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C67" s="2">
         <v>3.2099999999999998E-7</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C68" s="2">
         <v>250000</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    <row r="69" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C69" s="8">
         <v>4.4999999999999999E-4</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E69" s="10" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add VEGF-B and PlGF concentration to parameter list
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5805CB-F9CB-2C4B-865C-F7A66706C566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041A7EDD-25D4-A149-BDAB-24A4FCA52414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="162">
   <si>
     <t>Parameter</t>
   </si>
@@ -510,6 +510,18 @@
   </si>
   <si>
     <t>Concentration of VEGFR1:NRP1</t>
+  </si>
+  <si>
+    <t>VB</t>
+  </si>
+  <si>
+    <t>Pl</t>
+  </si>
+  <si>
+    <t>Concentration of VEGF-B</t>
+  </si>
+  <si>
+    <t>Concentration of PlGF</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DEB865-22A6-6340-B754-943FBB9E2F98}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,10 +1147,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="C3" s="2">
         <v>1.0000000000000001E-9</v>
@@ -1152,10 +1164,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>35</v>
+        <v>159</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="C4" s="2">
         <v>1.0000000000000001E-9</v>
@@ -1169,10 +1181,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2">
         <v>1.0000000000000001E-9</v>
@@ -1186,134 +1198,134 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C8" s="2">
         <f>802*2</f>
         <v>1604</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C9" s="2">
         <f>2047*2</f>
         <v>4094</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C10" s="2">
         <f>22045*2</f>
         <v>44090</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C11" s="2">
         <f>2501*2</f>
         <v>5002</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C12" s="2">
         <f>2670*2</f>
         <v>5340</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -1327,10 +1339,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -1344,10 +1356,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -1361,10 +1373,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
@@ -1378,10 +1390,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -1395,10 +1407,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -1412,10 +1424,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -1429,10 +1441,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -1446,10 +1458,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -1463,10 +1475,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C22" s="2">
         <v>0</v>
@@ -1480,10 +1492,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
@@ -1497,10 +1509,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
@@ -1514,10 +1526,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -1531,10 +1543,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
@@ -1548,10 +1560,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
@@ -1565,10 +1577,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
@@ -1582,10 +1594,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -1599,47 +1611,47 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>2</v>
+        <v>143</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="C30" s="2">
-        <v>11370000</v>
+        <v>0</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="C31" s="2">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="2">
-        <v>4650000</v>
+        <v>11370000</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>45</v>
@@ -1650,13 +1662,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2">
-        <v>7.6999999999999996E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>44</v>
@@ -1667,13 +1679,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>73</v>
+        <v>3</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C34" s="2">
-        <v>1260000</v>
+        <v>4650000</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>45</v>
@@ -1684,13 +1696,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>82</v>
+        <v>18</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="C35" s="2">
-        <v>3.48E-3</v>
+        <v>7.6999999999999996E-4</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>44</v>
@@ -1701,61 +1713,61 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>74</v>
+        <v>4</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="C36" s="2">
-        <v>100000000000000</v>
+        <v>1260000</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>19</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="C37" s="2">
-        <v>1E-3</v>
+        <v>3.48E-3</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="2">
-        <v>31000000000000</v>
+        <v>100000000000000</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="2">
         <v>1E-3</v>
@@ -1764,52 +1776,52 @@
         <v>44</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="C40" s="2">
-        <v>158000</v>
+        <v>31000000000000</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>107</v>
+        <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="C41" s="2">
-        <v>9.145E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C42" s="2">
-        <v>126000</v>
+        <v>158000</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>45</v>
@@ -1820,13 +1832,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C43" s="2">
-        <v>1.94E-4</v>
+        <v>9.145E-5</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>44</v>
@@ -1837,13 +1849,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C44" s="2">
-        <v>57900</v>
+        <v>126000</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>45</v>
@@ -1854,13 +1866,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="2">
-        <v>2.6900000000000001E-6</v>
+        <v>1.94E-4</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>44</v>
@@ -1871,81 +1883,81 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C46" s="2">
-        <v>10000</v>
+        <v>57900</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C47" s="2">
-        <v>1E-3</v>
+        <v>2.6900000000000001E-6</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="C48" s="2">
-        <v>1100</v>
+        <v>10000</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="C49" s="2">
-        <v>2.6999999999999999E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C50" s="2">
-        <v>12000</v>
+        <v>1100</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>45</v>
@@ -1956,13 +1968,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C51" s="2">
-        <v>3.9999999999999998E-6</v>
+        <v>2.6999999999999999E-5</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>44</v>
@@ -1973,47 +1985,47 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C52" s="2">
-        <v>204000</v>
+        <v>12000</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C53" s="2">
-        <v>3.035E-4</v>
+        <v>3.9999999999999998E-6</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C54" s="2">
-        <v>162000</v>
+        <v>204000</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>45</v>
@@ -2024,13 +2036,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C55" s="2">
-        <v>3.8299999999999999E-4</v>
+        <v>3.035E-4</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>44</v>
@@ -2041,13 +2053,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C56" s="2">
-        <v>169000</v>
+        <v>162000</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>45</v>
@@ -2058,13 +2070,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C57" s="2">
-        <v>3.77E-4</v>
+        <v>3.8299999999999999E-4</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>44</v>
@@ -2075,13 +2087,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C58" s="2">
-        <v>214000</v>
+        <v>169000</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>45</v>
@@ -2092,13 +2104,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C59" s="2">
-        <v>5.8100000000000001E-3</v>
+        <v>3.77E-4</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>44</v>
@@ -2109,101 +2121,101 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C60" s="2">
-        <v>1300</v>
+        <v>214000</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C61" s="2">
-        <v>2.8999999999999998E-3</v>
+        <v>5.8100000000000001E-3</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1300</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C64" s="2">
         <f>(336000+325000)/2</f>
         <v>330500</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E64" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C65" s="2">
         <f>(0.000604+0.000905)/2</f>
         <v>7.5449999999999996E-4</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" s="2">
-        <v>219000</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" s="2">
-        <v>3.0300000000000001E-5</v>
-      </c>
       <c r="D65" s="3" t="s">
         <v>44</v>
       </c>
@@ -2213,13 +2225,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C66" s="2">
-        <v>173000</v>
+        <v>219000</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>45</v>
@@ -2230,13 +2242,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C67" s="2">
-        <v>3.2099999999999998E-7</v>
+        <v>3.0300000000000001E-5</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>44</v>
@@ -2247,35 +2259,69 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C68" s="2">
-        <v>250000</v>
+        <v>173000</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E68" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="2">
+        <v>3.2099999999999998E-7</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="2">
+        <v>250000</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+    <row r="71" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="8">
+      <c r="C71" s="8">
         <v>4.4999999999999999E-4</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D71" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E71" s="10" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the number of digits to be specified
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661C70F7-67C1-2A4A-9F9D-85274F7C5C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C6430E-5B68-DF4B-A64C-2A621A821F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -528,6 +528,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -734,7 +737,6 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -744,7 +746,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -762,6 +763,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DEB865-22A6-6340-B754-943FBB9E2F98}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1112,1216 +1115,1216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="14">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="14">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="14">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="14">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="14">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="14">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="14">
         <f>802*2</f>
         <v>1604</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="14">
         <f>2047*2</f>
         <v>4094</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="14">
         <f>22045*2</f>
         <v>44090</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="14">
         <f>2501*2</f>
         <v>5002</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="14">
         <f>2670*2</f>
         <v>5340</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="14">
         <v>0</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="14">
         <v>0</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="14">
         <v>0</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="14">
         <v>0</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="14">
         <v>0</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="14">
         <v>0</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="D18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="14">
         <v>0</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="14">
         <v>0</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="D20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="14">
         <v>0</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="D21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="14">
         <v>0</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="14">
         <v>0</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="14">
         <v>0</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="D24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="14">
         <v>0</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="D25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>139</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="14">
         <v>0</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="14">
         <v>0</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="D27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="14">
         <v>0</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="D28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="14">
         <v>0</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="14">
         <v>0</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="D30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="14">
         <v>0</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="D31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="14">
         <v>11370000</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="14">
         <v>1E-4</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="14">
         <v>4650000</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="14">
         <v>7.6999999999999996E-4</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="14">
         <v>1260000</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="14">
         <v>3.48E-3</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="14">
         <v>100000000000000</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="14">
         <v>31000000000000</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="14">
         <v>158000</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="14">
         <v>9.145E-5</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="14">
         <v>126000</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="14">
         <v>1.94E-4</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="14">
         <v>57900</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="14">
         <v>2.6900000000000001E-6</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="14">
         <v>10000</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="14">
         <v>1100</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="14">
         <v>2.6999999999999999E-5</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="14">
         <v>12000</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="14">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="14">
         <v>204000</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="14">
         <v>3.035E-4</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="14">
         <v>162000</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="14">
         <v>3.8299999999999999E-4</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="14">
         <v>169000</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="14">
         <v>3.77E-4</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="14">
         <v>214000</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E60" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="14">
         <v>5.8100000000000003E-4</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="14">
         <v>1300</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="14">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="14">
         <f>(336000+325000)/2</f>
         <v>330500</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E64" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="14">
         <f>(0.000604+0.000905)/2</f>
         <v>7.5449999999999996E-4</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="14">
         <v>219000</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="14">
         <v>3.0300000000000001E-5</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="14">
         <v>173000</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="14">
         <v>3.2099999999999998E-7</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="14">
         <v>250000</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="8">
+      <c r="C71" s="15">
         <v>4.4999999999999999E-4</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D71" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="E71" s="8" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. set concentration of species except VA, Pl, R1, and R2 and 2. change VA and Pl concentration to 2.22 µM
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F5938-4F69-D14D-B5D4-1F8C87B64CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{106437AF-5372-3E41-A1B9-19505D548F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
+    <workbookView xWindow="14040" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1156,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1207,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1224,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1276,7 +1276,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>44090</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1293,7 +1293,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>5001</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1310,7 +1310,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>5341</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
set PlGF concentration as 0
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F5938-4F69-D14D-B5D4-1F8C87B64CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39656F0B-1D32-444E-9ED7-A7E55DA1C2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Revert "1. set concentration of species except VA, Pl, R1, and R2 and 2. change VA and Pl concentration to 2.22 µM"
This reverts commit 3198ec71181c094bc71047c5e880353900bad246.
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/x-family_membrane/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{106437AF-5372-3E41-A1B9-19505D548F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F5938-4F69-D14D-B5D4-1F8C87B64CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1156,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1207,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1224,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1276,7 +1276,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>0</v>
+        <v>44090</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1293,7 +1293,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>0</v>
+        <v>5001</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1310,7 +1310,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>0</v>
+        <v>5341</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Revert "Revert "1. set concentration of species except VA, Pl, R1, and R2 and 2. change VA and Pl concentration to 2.22 µM""
This reverts commit c462d53f15308679b9cf889ad579ed220772b874.
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F5938-4F69-D14D-B5D4-1F8C87B64CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{106437AF-5372-3E41-A1B9-19505D548F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
+    <workbookView xWindow="14040" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1156,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1207,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1224,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1276,7 +1276,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>44090</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1293,7 +1293,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>5001</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1310,7 +1310,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>5341</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
use rounded receptor densities (confirmed by Cheri) and reduce # of significant digits of binding rates to 2, which is measured by Shobhan
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/x-family_membrane/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{106437AF-5372-3E41-A1B9-19505D548F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504F2541-9C13-244B-A64B-4CF9008473F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -765,6 +765,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DEB865-22A6-6340-B754-943FBB9E2F98}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,8 +1242,8 @@
         <v>66</v>
       </c>
       <c r="C8" s="14">
-        <f>1604</f>
-        <v>1604</v>
+        <f>1600</f>
+        <v>1600</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>43</v>
@@ -1259,7 +1260,8 @@
         <v>67</v>
       </c>
       <c r="C9" s="14">
-        <v>4095</v>
+        <f>4100</f>
+        <v>4100</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>43</v>
@@ -1649,8 +1651,8 @@
       <c r="B32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="14">
-        <v>11370000</v>
+      <c r="C32" s="16">
+        <v>11000000</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>45</v>
@@ -1666,7 +1668,7 @@
       <c r="B33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="16">
         <v>1E-4</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1683,8 +1685,8 @@
       <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="14">
-        <v>4650000</v>
+      <c r="C34" s="16">
+        <v>4600000</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>45</v>
@@ -1700,7 +1702,7 @@
       <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="16">
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1717,8 +1719,8 @@
       <c r="B36" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="14">
-        <v>1260000</v>
+      <c r="C36" s="16">
+        <v>1300000</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>45</v>
@@ -1734,8 +1736,8 @@
       <c r="B37" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="14">
-        <v>3.48E-3</v>
+      <c r="C37" s="16">
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>44</v>
@@ -1751,7 +1753,7 @@
       <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="16">
         <v>100000000000000</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -1768,7 +1770,7 @@
       <c r="B39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="16">
         <v>1E-3</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1785,7 +1787,7 @@
       <c r="B40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="16">
         <v>31000000000000</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -1802,7 +1804,7 @@
       <c r="B41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="16">
         <v>1E-3</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -1819,7 +1821,7 @@
       <c r="B42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="16">
         <v>158000</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -1836,8 +1838,8 @@
       <c r="B43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="14">
-        <v>9.145E-5</v>
+      <c r="C43" s="16">
+        <v>9.1500000000000001E-5</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>44</v>
@@ -1853,7 +1855,7 @@
       <c r="B44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="16">
         <v>126000</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -1870,7 +1872,7 @@
       <c r="B45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="16">
         <v>1.94E-4</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -1887,7 +1889,7 @@
       <c r="B46" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="16">
         <v>57900</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -1904,7 +1906,7 @@
       <c r="B47" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="16">
         <v>2.6900000000000001E-6</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -1921,7 +1923,7 @@
       <c r="B48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="16">
         <v>10000</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -1938,7 +1940,7 @@
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="16">
         <v>1E-3</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -1955,7 +1957,7 @@
       <c r="B50" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="14">
+      <c r="C50" s="16">
         <v>1100</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -1972,7 +1974,7 @@
       <c r="B51" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="16">
         <v>2.6999999999999999E-5</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -1989,7 +1991,7 @@
       <c r="B52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52" s="16">
         <v>12000</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2006,7 +2008,7 @@
       <c r="B53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="16">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -2023,7 +2025,7 @@
       <c r="B54" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="16">
         <v>204000</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2040,8 +2042,8 @@
       <c r="B55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="14">
-        <v>3.035E-4</v>
+      <c r="C55" s="16">
+        <v>3.0400000000000002E-4</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>44</v>
@@ -2057,7 +2059,7 @@
       <c r="B56" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="16">
         <v>162000</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -2074,7 +2076,7 @@
       <c r="B57" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="16">
         <v>3.8299999999999999E-4</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -2091,7 +2093,7 @@
       <c r="B58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C58" s="14">
+      <c r="C58" s="16">
         <v>169000</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -2108,7 +2110,7 @@
       <c r="B59" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C59" s="14">
+      <c r="C59" s="16">
         <v>3.77E-4</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -2125,7 +2127,7 @@
       <c r="B60" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="14">
+      <c r="C60" s="16">
         <v>214000</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -2142,7 +2144,7 @@
       <c r="B61" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="14">
+      <c r="C61" s="16">
         <v>5.8100000000000003E-4</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -2159,7 +2161,7 @@
       <c r="B62" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C62" s="14">
+      <c r="C62" s="16">
         <v>1300</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -2176,7 +2178,7 @@
       <c r="B63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63" s="16">
         <v>2.8999999999999998E-3</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -2193,9 +2195,8 @@
       <c r="B64" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="14">
-        <f>(336000+325000)/2</f>
-        <v>330500</v>
+      <c r="C64" s="16">
+        <v>331000</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>45</v>
@@ -2211,9 +2212,8 @@
       <c r="B65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="14">
-        <f>(0.000604+0.000905)/2</f>
-        <v>7.5449999999999996E-4</v>
+      <c r="C65" s="16">
+        <v>7.5500000000000003E-4</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>44</v>
@@ -2229,7 +2229,7 @@
       <c r="B66" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C66" s="16">
         <v>219000</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -2246,7 +2246,7 @@
       <c r="B67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C67" s="16">
         <v>3.0300000000000001E-5</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -2263,7 +2263,7 @@
       <c r="B68" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="14">
+      <c r="C68" s="16">
         <v>173000</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -2280,7 +2280,7 @@
       <c r="B69" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="14">
+      <c r="C69" s="16">
         <v>3.2099999999999998E-7</v>
       </c>
       <c r="D69" s="2" t="s">

</xml_diff>

<commit_message>
restore the ligand concentration (1 nM) and use rounded receptor densities, which is confirmed by Cheri
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504F2541-9C13-244B-A64B-4CF9008473F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DE6723-31EE-9144-AED8-E086239F1B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -765,7 +765,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DEB865-22A6-6340-B754-943FBB9E2F98}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C69"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1157,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1174,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1191,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1208,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1225,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1278,7 +1277,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>0</v>
+        <v>44100</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1295,7 +1294,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1312,7 +1311,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>0</v>
+        <v>5300</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>
@@ -1651,7 +1650,7 @@
       <c r="B32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="14">
         <v>11000000</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1668,7 +1667,7 @@
       <c r="B33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="14">
         <v>1E-4</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1685,7 +1684,7 @@
       <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="14">
         <v>4600000</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -1702,7 +1701,7 @@
       <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="14">
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1719,7 +1718,7 @@
       <c r="B36" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="14">
         <v>1300000</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -1736,7 +1735,7 @@
       <c r="B37" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="14">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1753,7 +1752,7 @@
       <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="14">
         <v>100000000000000</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -1770,7 +1769,7 @@
       <c r="B39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="14">
         <v>1E-3</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1787,7 +1786,7 @@
       <c r="B40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="14">
         <v>31000000000000</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -1804,7 +1803,7 @@
       <c r="B41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="14">
         <v>1E-3</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -1821,7 +1820,7 @@
       <c r="B42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="14">
         <v>158000</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -1838,7 +1837,7 @@
       <c r="B43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="16">
+      <c r="C43" s="14">
         <v>9.1500000000000001E-5</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -1855,7 +1854,7 @@
       <c r="B44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44" s="14">
         <v>126000</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -1872,7 +1871,7 @@
       <c r="B45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45" s="14">
         <v>1.94E-4</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -1889,7 +1888,7 @@
       <c r="B46" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="16">
+      <c r="C46" s="14">
         <v>57900</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -1906,7 +1905,7 @@
       <c r="B47" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="16">
+      <c r="C47" s="14">
         <v>2.6900000000000001E-6</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -1923,7 +1922,7 @@
       <c r="B48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="14">
         <v>10000</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -1940,7 +1939,7 @@
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="16">
+      <c r="C49" s="14">
         <v>1E-3</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -1957,7 +1956,7 @@
       <c r="B50" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50" s="14">
         <v>1100</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -1974,7 +1973,7 @@
       <c r="B51" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="16">
+      <c r="C51" s="14">
         <v>2.6999999999999999E-5</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -1991,7 +1990,7 @@
       <c r="B52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C52" s="14">
         <v>12000</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2008,7 +2007,7 @@
       <c r="B53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="16">
+      <c r="C53" s="14">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -2025,7 +2024,7 @@
       <c r="B54" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="16">
+      <c r="C54" s="14">
         <v>204000</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2042,7 +2041,7 @@
       <c r="B55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="16">
+      <c r="C55" s="14">
         <v>3.0400000000000002E-4</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -2059,7 +2058,7 @@
       <c r="B56" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="16">
+      <c r="C56" s="14">
         <v>162000</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -2076,7 +2075,7 @@
       <c r="B57" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="16">
+      <c r="C57" s="14">
         <v>3.8299999999999999E-4</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -2093,7 +2092,7 @@
       <c r="B58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C58" s="16">
+      <c r="C58" s="14">
         <v>169000</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -2110,7 +2109,7 @@
       <c r="B59" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C59" s="14">
         <v>3.77E-4</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -2127,7 +2126,7 @@
       <c r="B60" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="16">
+      <c r="C60" s="14">
         <v>214000</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -2144,7 +2143,7 @@
       <c r="B61" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="16">
+      <c r="C61" s="14">
         <v>5.8100000000000003E-4</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -2161,7 +2160,7 @@
       <c r="B62" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C62" s="16">
+      <c r="C62" s="14">
         <v>1300</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -2178,7 +2177,7 @@
       <c r="B63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="16">
+      <c r="C63" s="14">
         <v>2.8999999999999998E-3</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -2195,7 +2194,7 @@
       <c r="B64" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="16">
+      <c r="C64" s="14">
         <v>331000</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -2212,7 +2211,7 @@
       <c r="B65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="16">
+      <c r="C65" s="14">
         <v>7.5500000000000003E-4</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -2229,7 +2228,7 @@
       <c r="B66" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="16">
+      <c r="C66" s="14">
         <v>219000</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -2246,7 +2245,7 @@
       <c r="B67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C67" s="16">
+      <c r="C67" s="14">
         <v>3.0300000000000001E-5</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -2263,7 +2262,7 @@
       <c r="B68" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="16">
+      <c r="C68" s="14">
         <v>173000</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -2280,7 +2279,7 @@
       <c r="B69" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="16">
+      <c r="C69" s="14">
         <v>3.2099999999999998E-7</v>
       </c>
       <c r="D69" s="2" t="s">

</xml_diff>

<commit_message>
change PlGF concentration from 1 nM to 0 nM
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DE6723-31EE-9144-AED8-E086239F1B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89843520-0EB9-6648-87DE-957D70D19979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DEB865-22A6-6340-B754-943FBB9E2F98}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
restore PlGF concentration from 0 nM to 1 nM
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89843520-0EB9-6648-87DE-957D70D19979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CA997B-F17E-2F4B-A2CA-DB40D6F5A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
set PlGF concentration as 0 nM
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CA997B-F17E-2F4B-A2CA-DB40D6F5A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFC5B9D-6214-814B-AAF4-58E22835A553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Revert "set PlGF concentration as 0 nM"
This reverts commit 10d5f628e308638528d73843fa5f95f0a3642aaf.
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFC5B9D-6214-814B-AAF4-58E22835A553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CA997B-F17E-2F4B-A2CA-DB40D6F5A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
set VEGF-A and PlGF concentration as 2.22 µM and set concentrations of other species as 0
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CA997B-F17E-2F4B-A2CA-DB40D6F5A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE4618E-63F0-A34B-896E-F5BAF1ABD912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1156,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1207,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1224,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1277,7 +1277,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>44100</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1294,7 +1294,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1311,7 +1311,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>5300</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Revert "set VEGF-A and PlGF concentration as 2.22 µM and set concentrations of other species as 0"
This reverts commit bdd9181c81f1489fd67633be86d38e613ca30dde.
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE4618E-63F0-A34B-896E-F5BAF1ABD912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CA997B-F17E-2F4B-A2CA-DB40D6F5A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1156,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1207,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1224,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1277,7 +1277,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>0</v>
+        <v>44100</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1294,7 +1294,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1311,7 +1311,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>0</v>
+        <v>5300</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
set free PlGF concentration as 0
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CA997B-F17E-2F4B-A2CA-DB40D6F5A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5075193-C76F-1C4D-B497-CB39300B0F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
change the concentration of VEGF-A and PlGF to 2.22 µM and set NRP1, PDGFRalpha, and PDGFRbeta concentrations as 0
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3540A67-32D1-1A4B-9A02-932E03DA882C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C340E58-8DEF-1941-8C1C-C5D71BB8AF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1156,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1207,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1224,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1277,7 +1277,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>44100</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1294,7 +1294,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1311,7 +1311,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>5300</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Revert "change the concentration of VEGF-A and PlGF to 2.22 µM and set NRP1, PDGFRalpha, and PDGFRbeta concentrations as 0"
This reverts commit 73a6872a1054dfb0dffe09b7d37e88a7ab066a97.
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C340E58-8DEF-1941-8C1C-C5D71BB8AF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3540A67-32D1-1A4B-9A02-932E03DA882C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1156,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="14">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1207,7 +1207,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1224,7 +1224,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="14">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1277,7 +1277,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="14">
-        <v>0</v>
+        <v>44100</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1294,7 +1294,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1311,7 +1311,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="14">
-        <v>0</v>
+        <v>5300</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Revert "set PlGF concentration as 0"
This reverts commit 4c115ea7b8823f3fb769eed4ef0b70824083cf07.
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3816B0-311A-3045-8A9A-A94E97764CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E597451D-E468-F749-9CF1-5E19066CFF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E32" sqref="E32:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1167,7 @@
         <v>154</v>
       </c>
       <c r="C4" s="12">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
change concentration of VEGF-A and PlGF to 2.22 µM and set receptors' concentration (except for VEGFRs) as 0
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E597451D-E468-F749-9CF1-5E19066CFF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922370E2-28E3-1D4E-9543-1C6B79F14285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32:E37"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,7 +1133,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="12">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1150,7 +1150,7 @@
         <v>153</v>
       </c>
       <c r="C3" s="12">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1167,7 +1167,7 @@
         <v>154</v>
       </c>
       <c r="C4" s="12">
-        <v>1.0000000000000001E-9</v>
+        <v>2.2199999999999999E-6</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1184,7 +1184,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="12">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1201,7 +1201,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="12">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1218,7 +1218,7 @@
         <v>58</v>
       </c>
       <c r="C7" s="12">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1271,7 +1271,7 @@
         <v>61</v>
       </c>
       <c r="C10" s="12">
-        <v>44100</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1288,7 +1288,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1305,7 +1305,7 @@
         <v>63</v>
       </c>
       <c r="C12" s="12">
-        <v>5300</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Revert "change concentration of VEGF-A and PlGF to 2.22 µM and set receptors' concentration (except for VEGFRs) as 0"
This reverts commit 934b67c66e327b059753aab6f289f56d0aaeb34d.
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922370E2-28E3-1D4E-9543-1C6B79F14285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E597451D-E468-F749-9CF1-5E19066CFF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{ACFAE212-61DD-9F46-B940-C448A07487F4}"/>
   </bookViews>
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E32" sqref="E32:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,7 +1133,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="12">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1150,7 +1150,7 @@
         <v>153</v>
       </c>
       <c r="C3" s="12">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -1167,7 +1167,7 @@
         <v>154</v>
       </c>
       <c r="C4" s="12">
-        <v>2.2199999999999999E-6</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -1184,7 +1184,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="12">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>46</v>
@@ -1201,7 +1201,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="12">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>46</v>
@@ -1218,7 +1218,7 @@
         <v>58</v>
       </c>
       <c r="C7" s="12">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
@@ -1271,7 +1271,7 @@
         <v>61</v>
       </c>
       <c r="C10" s="12">
-        <v>0</v>
+        <v>44100</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
@@ -1288,7 +1288,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
@@ -1305,7 +1305,7 @@
         <v>63</v>
       </c>
       <c r="C12" s="12">
-        <v>0</v>
+        <v>5300</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>43</v>

</xml_diff>